<commit_message>
Added results to ItemBasedResults.xlsx
</commit_message>
<xml_diff>
--- a/Report/Results/ItemBasedResults.xlsx
+++ b/Report/Results/ItemBasedResults.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ShaownS/PycharmProjects/CSC791MLUAS_Project/Report/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meneal/Documents/gits/spr16/CSC791MLUAS_Project/Report/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="19780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overall" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>NumRecs</t>
   </si>
   <si>
     <t>SuccessRate</t>
+  </si>
+  <si>
+    <t>Item Based</t>
+  </si>
+  <si>
+    <t>User Based (10 Users)</t>
+  </si>
+  <si>
+    <t>User Based (20 Users)</t>
+  </si>
+  <si>
+    <t>Baseline</t>
   </si>
 </sst>
 </file>
@@ -74,9 +84,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -92,6 +108,553 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Overall</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Comparison of Algorithms</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overall!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Item Based</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Overall!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2766</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5429</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overall!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>User Based (10 Users)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Overall!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1776</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.345</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4628</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overall!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>User Based (20 Users)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Overall!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1918</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4771</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5971</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overall!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Overall!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.141</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7064</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.873</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2074202880"/>
+        <c:axId val="-2077013520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2074202880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2077013520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2077013520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2074202880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -249,11 +812,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2104451152"/>
-        <c:axId val="2134591712"/>
+        <c:axId val="-2118820688"/>
+        <c:axId val="-2121136912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2104451152"/>
+        <c:axId val="-2118820688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +922,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134591712"/>
+        <c:crossAx val="-2121136912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -367,7 +930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134591712"/>
+        <c:axId val="-2121136912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +1003,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104451152"/>
+        <c:crossAx val="-2118820688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -490,6 +1053,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
   <a:schemeClr val="dk1"/>
   <cs:variation>
@@ -1019,7 +1622,545 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1317,10 +2458,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.27660000000000001</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.54290000000000005</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.62450000000000006</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.17760000000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.39939999999999998</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.46279999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.1918</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.47710000000000002</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.41310000000000002</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.59709999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.5222</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>